<commit_message>
final commit 5 nov
</commit_message>
<xml_diff>
--- a/excelfile.xlsx
+++ b/excelfile.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>sr no</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>akash patil</t>
+  </si>
+  <si>
+    <t>Tanmay Bore</t>
   </si>
 </sst>
 </file>
@@ -1220,74 +1223,74 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="5.85714285714286" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="21.5714285714286" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="5.85714285714286"/>
+    <col min="2" max="2" customWidth="true" width="16.0"/>
+    <col min="3" max="3" customWidth="true" width="21.5714285714286"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>8</v>
       </c>
     </row>

</xml_diff>